<commit_message>
Allocation fixes and generated excel files using its data
</commit_message>
<xml_diff>
--- a/A2/output/masterGenHistory.xlsx
+++ b/A2/output/masterGenHistory.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\tag\Documents\GitHub\CS4341\A2\output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Documents\GitHub\CS4341\A2\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -159,9 +159,12 @@
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -171,12 +174,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -288,7 +288,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.75</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -303,7 +303,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0</c:v>
@@ -318,22 +318,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>14</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>7.25</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>9</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>10.75</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>0</c:v>
@@ -354,46 +354,46 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>11</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>7.25</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>5.25</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="34">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>5.25</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>14</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>8.75</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>7.25</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="43">
                   <c:v>0</c:v>
@@ -402,40 +402,40 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="48">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>9.75</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="51">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>5.25</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="53">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>7.25</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="55">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>7.25</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="57">
                   <c:v>0</c:v>
@@ -444,13 +444,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>14.5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="60">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>50</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="62">
                   <c:v>0</c:v>
@@ -899,11 +899,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="200024728"/>
-        <c:axId val="200021200"/>
+        <c:axId val="441381736"/>
+        <c:axId val="441378992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="200024728"/>
+        <c:axId val="441381736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -946,7 +946,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="200021200"/>
+        <c:crossAx val="441378992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -954,7 +954,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="200021200"/>
+        <c:axId val="441378992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1005,7 +1005,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="200024728"/>
+        <c:crossAx val="441381736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1940,45 +1940,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X64"/>
+  <dimension ref="A1:X90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="AA14" sqref="AA14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2:S64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="E1" s="1" t="s">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="E1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="I1" s="1" t="s">
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="I1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="M1" s="1" t="s">
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="M1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="Q1" s="1" t="s">
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="Q1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="V1" s="2" t="s">
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="V1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="W1" s="3"/>
-      <c r="X1" s="4"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="9"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -2026,15 +2026,15 @@
       <c r="S2">
         <v>0</v>
       </c>
-      <c r="V2" s="5">
+      <c r="V2" s="1">
         <f>AVERAGE(A2,E2,I2,M2)</f>
         <v>0</v>
       </c>
-      <c r="W2" s="6">
+      <c r="W2" s="2">
         <f>AVERAGE(B2,F2,J2,N2)</f>
         <v>0</v>
       </c>
-      <c r="X2" s="7">
+      <c r="X2" s="3">
         <f>AVERAGE(C2,G2,K2,O2)</f>
         <v>0</v>
       </c>
@@ -2085,15 +2085,15 @@
       <c r="S3">
         <v>0</v>
       </c>
-      <c r="V3" s="5">
+      <c r="V3" s="1">
         <f t="shared" ref="V3:V64" si="0">AVERAGE(A3,E3,I3,M3)</f>
         <v>0</v>
       </c>
-      <c r="W3" s="6">
+      <c r="W3" s="2">
         <f t="shared" ref="W3:W64" si="1">AVERAGE(B3,F3,J3,N3)</f>
         <v>0</v>
       </c>
-      <c r="X3" s="7">
+      <c r="X3" s="3">
         <f t="shared" ref="X3:X64" si="2">AVERAGE(C3,G3,K3,O3)</f>
         <v>0</v>
       </c>
@@ -2144,15 +2144,15 @@
       <c r="S4">
         <v>0</v>
       </c>
-      <c r="V4" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W4" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X4" s="7">
+      <c r="V4" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W4" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X4" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2203,15 +2203,15 @@
       <c r="S5">
         <v>0</v>
       </c>
-      <c r="V5" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W5" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X5" s="7">
+      <c r="V5" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W5" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X5" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2262,15 +2262,15 @@
       <c r="S6">
         <v>0</v>
       </c>
-      <c r="V6" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W6" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X6" s="7">
+      <c r="V6" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W6" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X6" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2321,15 +2321,15 @@
       <c r="S7">
         <v>0</v>
       </c>
-      <c r="V7" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W7" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X7" s="7">
+      <c r="V7" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W7" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X7" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2380,22 +2380,22 @@
       <c r="S8">
         <v>0</v>
       </c>
-      <c r="V8" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W8" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X8" s="7">
+      <c r="V8" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W8" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X8" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -2439,15 +2439,15 @@
       <c r="S9">
         <v>0</v>
       </c>
-      <c r="V9" s="5">
-        <f t="shared" si="0"/>
-        <v>9.75</v>
-      </c>
-      <c r="W9" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X9" s="7">
+      <c r="V9" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W9" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X9" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2498,15 +2498,15 @@
       <c r="S10">
         <v>0</v>
       </c>
-      <c r="V10" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W10" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X10" s="7">
+      <c r="V10" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W10" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X10" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2557,15 +2557,15 @@
       <c r="S11">
         <v>0</v>
       </c>
-      <c r="V11" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W11" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X11" s="7">
+      <c r="V11" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W11" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X11" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2616,15 +2616,15 @@
       <c r="S12">
         <v>0</v>
       </c>
-      <c r="V12" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W12" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X12" s="7">
+      <c r="V12" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W12" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X12" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2675,15 +2675,15 @@
       <c r="S13">
         <v>0</v>
       </c>
-      <c r="V13" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W13" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X13" s="7">
+      <c r="V13" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W13" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X13" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2699,7 +2699,7 @@
         <v>0</v>
       </c>
       <c r="E14">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -2734,15 +2734,15 @@
       <c r="S14">
         <v>0</v>
       </c>
-      <c r="V14" s="5">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="W14" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X14" s="7">
+      <c r="V14" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W14" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X14" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2793,15 +2793,15 @@
       <c r="S15">
         <v>0</v>
       </c>
-      <c r="V15" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W15" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X15" s="7">
+      <c r="V15" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W15" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X15" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2852,15 +2852,15 @@
       <c r="S16">
         <v>0</v>
       </c>
-      <c r="V16" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W16" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X16" s="7">
+      <c r="V16" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W16" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X16" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2911,15 +2911,15 @@
       <c r="S17">
         <v>0</v>
       </c>
-      <c r="V17" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W17" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X17" s="7">
+      <c r="V17" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W17" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X17" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2970,15 +2970,15 @@
       <c r="S18">
         <v>0</v>
       </c>
-      <c r="V18" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W18" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X18" s="7">
+      <c r="V18" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W18" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X18" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2994,7 +2994,7 @@
         <v>0</v>
       </c>
       <c r="E19">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -3029,15 +3029,15 @@
       <c r="S19">
         <v>0</v>
       </c>
-      <c r="V19" s="5">
-        <f t="shared" si="0"/>
-        <v>3.5</v>
-      </c>
-      <c r="W19" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X19" s="7">
+      <c r="V19" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W19" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X19" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3062,7 +3062,7 @@
         <v>0</v>
       </c>
       <c r="I20">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="J20">
         <v>0</v>
@@ -3071,7 +3071,7 @@
         <v>0</v>
       </c>
       <c r="M20">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="N20">
         <v>0</v>
@@ -3088,15 +3088,15 @@
       <c r="S20">
         <v>0</v>
       </c>
-      <c r="V20" s="5">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="W20" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X20" s="7">
+      <c r="V20" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W20" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X20" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3121,7 +3121,7 @@
         <v>0</v>
       </c>
       <c r="I21">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="J21">
         <v>0</v>
@@ -3147,22 +3147,22 @@
       <c r="S21">
         <v>0</v>
       </c>
-      <c r="V21" s="5">
-        <f t="shared" si="0"/>
-        <v>7.25</v>
-      </c>
-      <c r="W21" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X21" s="7">
+      <c r="V21" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W21" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X21" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -3180,7 +3180,7 @@
         <v>0</v>
       </c>
       <c r="I22">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="J22">
         <v>0</v>
@@ -3206,15 +3206,15 @@
       <c r="S22">
         <v>0</v>
       </c>
-      <c r="V22" s="5">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="W22" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X22" s="7">
+      <c r="V22" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W22" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X22" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3265,22 +3265,22 @@
       <c r="S23">
         <v>0</v>
       </c>
-      <c r="V23" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W23" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X23" s="7">
+      <c r="V23" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W23" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X23" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -3298,7 +3298,7 @@
         <v>0</v>
       </c>
       <c r="I24">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="J24">
         <v>0</v>
@@ -3324,15 +3324,15 @@
       <c r="S24">
         <v>0</v>
       </c>
-      <c r="V24" s="5">
-        <f t="shared" si="0"/>
-        <v>10.75</v>
-      </c>
-      <c r="W24" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X24" s="7">
+      <c r="V24" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W24" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X24" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3383,15 +3383,15 @@
       <c r="S25">
         <v>0</v>
       </c>
-      <c r="V25" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W25" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X25" s="7">
+      <c r="V25" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W25" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X25" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3442,15 +3442,15 @@
       <c r="S26">
         <v>0</v>
       </c>
-      <c r="V26" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W26" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X26" s="7">
+      <c r="V26" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W26" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X26" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3501,15 +3501,15 @@
       <c r="S27">
         <v>0</v>
       </c>
-      <c r="V27" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W27" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X27" s="7">
+      <c r="V27" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W27" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X27" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3560,15 +3560,15 @@
       <c r="S28">
         <v>0</v>
       </c>
-      <c r="V28" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W28" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X28" s="7">
+      <c r="V28" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W28" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X28" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3619,15 +3619,15 @@
       <c r="S29">
         <v>0</v>
       </c>
-      <c r="V29" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W29" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X29" s="7">
+      <c r="V29" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W29" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X29" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3678,15 +3678,15 @@
       <c r="S30">
         <v>0</v>
       </c>
-      <c r="V30" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W30" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X30" s="7">
+      <c r="V30" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W30" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X30" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3702,7 +3702,7 @@
         <v>0</v>
       </c>
       <c r="E31">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F31">
         <v>0</v>
@@ -3720,7 +3720,7 @@
         <v>0</v>
       </c>
       <c r="M31">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="N31">
         <v>0</v>
@@ -3737,15 +3737,15 @@
       <c r="S31">
         <v>0</v>
       </c>
-      <c r="V31" s="5">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="W31" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X31" s="7">
+      <c r="V31" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W31" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X31" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3796,15 +3796,15 @@
       <c r="S32">
         <v>0</v>
       </c>
-      <c r="V32" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W32" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X32" s="7">
+      <c r="V32" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W32" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X32" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3838,7 +3838,7 @@
         <v>0</v>
       </c>
       <c r="M33">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="N33">
         <v>0</v>
@@ -3855,15 +3855,15 @@
       <c r="S33">
         <v>0</v>
       </c>
-      <c r="V33" s="5">
-        <f t="shared" si="0"/>
-        <v>7.25</v>
-      </c>
-      <c r="W33" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X33" s="7">
+      <c r="V33" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W33" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X33" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3914,15 +3914,15 @@
       <c r="S34">
         <v>0</v>
       </c>
-      <c r="V34" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W34" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X34" s="7">
+      <c r="V34" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W34" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X34" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3938,7 +3938,7 @@
         <v>0</v>
       </c>
       <c r="E35">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="F35">
         <v>0</v>
@@ -3973,15 +3973,15 @@
       <c r="S35">
         <v>0</v>
       </c>
-      <c r="V35" s="5">
-        <f t="shared" si="0"/>
-        <v>5.25</v>
-      </c>
-      <c r="W35" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X35" s="7">
+      <c r="V35" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W35" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X35" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -4032,22 +4032,22 @@
       <c r="S36">
         <v>0</v>
       </c>
-      <c r="V36" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W36" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X36" s="7">
+      <c r="V36" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W36" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X36" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -4091,15 +4091,15 @@
       <c r="S37">
         <v>0</v>
       </c>
-      <c r="V37" s="5">
-        <f t="shared" si="0"/>
-        <v>5.25</v>
-      </c>
-      <c r="W37" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X37" s="7">
+      <c r="V37" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W37" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X37" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -4150,15 +4150,15 @@
       <c r="S38">
         <v>0</v>
       </c>
-      <c r="V38" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W38" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X38" s="7">
+      <c r="V38" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W38" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X38" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -4174,7 +4174,7 @@
         <v>0</v>
       </c>
       <c r="E39">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="F39">
         <v>0</v>
@@ -4192,7 +4192,7 @@
         <v>0</v>
       </c>
       <c r="M39">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="N39">
         <v>0</v>
@@ -4209,15 +4209,15 @@
       <c r="S39">
         <v>0</v>
       </c>
-      <c r="V39" s="5">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="W39" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X39" s="7">
+      <c r="V39" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W39" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X39" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -4268,22 +4268,22 @@
       <c r="S40">
         <v>0</v>
       </c>
-      <c r="V40" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W40" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X40" s="7">
+      <c r="V40" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W40" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X40" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -4292,7 +4292,7 @@
         <v>0</v>
       </c>
       <c r="E41">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="F41">
         <v>0</v>
@@ -4327,22 +4327,22 @@
       <c r="S41">
         <v>0</v>
       </c>
-      <c r="V41" s="5">
-        <f t="shared" si="0"/>
-        <v>8.75</v>
-      </c>
-      <c r="W41" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X41" s="7">
+      <c r="V41" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W41" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X41" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -4386,22 +4386,22 @@
       <c r="S42">
         <v>0</v>
       </c>
-      <c r="V42" s="5">
-        <f t="shared" si="0"/>
-        <v>7.25</v>
-      </c>
-      <c r="W42" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X42" s="7">
+      <c r="V42" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W42" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X42" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -4445,15 +4445,15 @@
       <c r="S43">
         <v>0</v>
       </c>
-      <c r="V43" s="5">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="W43" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X43" s="7">
+      <c r="V43" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W43" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X43" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -4487,7 +4487,7 @@
         <v>0</v>
       </c>
       <c r="M44">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="N44">
         <v>0</v>
@@ -4504,15 +4504,15 @@
       <c r="S44">
         <v>0</v>
       </c>
-      <c r="V44" s="5">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="W44" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X44" s="7">
+      <c r="V44" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W44" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X44" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -4563,15 +4563,15 @@
       <c r="S45">
         <v>0</v>
       </c>
-      <c r="V45" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W45" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X45" s="7">
+      <c r="V45" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W45" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X45" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -4622,15 +4622,15 @@
       <c r="S46">
         <v>0</v>
       </c>
-      <c r="V46" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W46" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X46" s="7">
+      <c r="V46" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W46" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X46" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -4646,7 +4646,7 @@
         <v>0</v>
       </c>
       <c r="E47">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F47">
         <v>0</v>
@@ -4681,15 +4681,15 @@
       <c r="S47">
         <v>0</v>
       </c>
-      <c r="V47" s="5">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="W47" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X47" s="7">
+      <c r="V47" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W47" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X47" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -4705,7 +4705,7 @@
         <v>0</v>
       </c>
       <c r="E48">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F48">
         <v>0</v>
@@ -4740,15 +4740,15 @@
       <c r="S48">
         <v>0</v>
       </c>
-      <c r="V48" s="5">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="W48" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X48" s="7">
+      <c r="V48" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W48" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X48" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -4764,7 +4764,7 @@
         <v>0</v>
       </c>
       <c r="E49">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F49">
         <v>0</v>
@@ -4791,7 +4791,7 @@
         <v>0</v>
       </c>
       <c r="Q49">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="R49">
         <v>0</v>
@@ -4799,15 +4799,15 @@
       <c r="S49">
         <v>0</v>
       </c>
-      <c r="V49" s="5">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="W49" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X49" s="7">
+      <c r="V49" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W49" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X49" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -4858,22 +4858,22 @@
       <c r="S50">
         <v>0</v>
       </c>
-      <c r="V50" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W50" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X50" s="7">
+      <c r="V50" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W50" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X50" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -4917,15 +4917,15 @@
       <c r="S51">
         <v>0</v>
       </c>
-      <c r="V51" s="5">
-        <f t="shared" si="0"/>
-        <v>9.75</v>
-      </c>
-      <c r="W51" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X51" s="7">
+      <c r="V51" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W51" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X51" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -4959,7 +4959,7 @@
         <v>0</v>
       </c>
       <c r="M52">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="N52">
         <v>0</v>
@@ -4976,15 +4976,15 @@
       <c r="S52">
         <v>0</v>
       </c>
-      <c r="V52" s="5">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="W52" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X52" s="7">
+      <c r="V52" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W52" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X52" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -5035,15 +5035,15 @@
       <c r="S53">
         <v>0</v>
       </c>
-      <c r="V53" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W53" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X53" s="7">
+      <c r="V53" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W53" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X53" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -5059,7 +5059,7 @@
         <v>0</v>
       </c>
       <c r="E54">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="F54">
         <v>0</v>
@@ -5094,15 +5094,15 @@
       <c r="S54">
         <v>0</v>
       </c>
-      <c r="V54" s="5">
-        <f t="shared" si="0"/>
-        <v>5.25</v>
-      </c>
-      <c r="W54" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X54" s="7">
+      <c r="V54" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W54" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X54" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -5153,15 +5153,15 @@
       <c r="S55">
         <v>0</v>
       </c>
-      <c r="V55" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W55" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X55" s="7">
+      <c r="V55" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W55" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X55" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -5195,7 +5195,7 @@
         <v>0</v>
       </c>
       <c r="M56">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="N56">
         <v>0</v>
@@ -5212,15 +5212,15 @@
       <c r="S56">
         <v>0</v>
       </c>
-      <c r="V56" s="5">
-        <f t="shared" si="0"/>
-        <v>7.25</v>
-      </c>
-      <c r="W56" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X56" s="7">
+      <c r="V56" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W56" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X56" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -5271,15 +5271,15 @@
       <c r="S57">
         <v>0</v>
       </c>
-      <c r="V57" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W57" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X57" s="7">
+      <c r="V57" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W57" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X57" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -5313,7 +5313,7 @@
         <v>0</v>
       </c>
       <c r="M58">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="N58">
         <v>0</v>
@@ -5330,15 +5330,15 @@
       <c r="S58">
         <v>0</v>
       </c>
-      <c r="V58" s="5">
-        <f t="shared" si="0"/>
-        <v>7.25</v>
-      </c>
-      <c r="W58" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X58" s="7">
+      <c r="V58" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W58" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X58" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -5389,15 +5389,15 @@
       <c r="S59">
         <v>0</v>
       </c>
-      <c r="V59" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W59" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X59" s="7">
+      <c r="V59" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W59" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X59" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -5448,22 +5448,22 @@
       <c r="S60">
         <v>0</v>
       </c>
-      <c r="V60" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W60" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X60" s="7">
+      <c r="V60" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W60" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X60" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="B61">
         <v>0</v>
@@ -5490,7 +5490,7 @@
         <v>0</v>
       </c>
       <c r="M61">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="N61">
         <v>0</v>
@@ -5507,15 +5507,15 @@
       <c r="S61">
         <v>0</v>
       </c>
-      <c r="V61" s="5">
-        <f t="shared" si="0"/>
-        <v>14.5</v>
-      </c>
-      <c r="W61" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X61" s="7">
+      <c r="V61" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W61" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X61" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -5566,22 +5566,22 @@
       <c r="S62">
         <v>0</v>
       </c>
-      <c r="V62" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W62" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X62" s="7">
+      <c r="V62" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W62" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X62" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="B63">
         <v>0</v>
@@ -5589,6 +5589,33 @@
       <c r="C63">
         <v>0</v>
       </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63">
+        <v>0</v>
+      </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
+      <c r="I63">
+        <v>0</v>
+      </c>
+      <c r="J63">
+        <v>0</v>
+      </c>
+      <c r="K63">
+        <v>0</v>
+      </c>
+      <c r="M63">
+        <v>0</v>
+      </c>
+      <c r="N63">
+        <v>0</v>
+      </c>
+      <c r="O63">
+        <v>0</v>
+      </c>
       <c r="Q63">
         <v>0</v>
       </c>
@@ -5598,15 +5625,15 @@
       <c r="S63">
         <v>0</v>
       </c>
-      <c r="V63" s="5">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="W63" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X63" s="7">
+      <c r="V63" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W63" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X63" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -5621,17 +5648,339 @@
       <c r="C64">
         <v>0</v>
       </c>
-      <c r="V64" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W64" s="9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X64" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="F64">
+        <v>0</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
+      </c>
+      <c r="I64">
+        <v>0</v>
+      </c>
+      <c r="J64">
+        <v>0</v>
+      </c>
+      <c r="K64">
+        <v>0</v>
+      </c>
+      <c r="M64">
+        <v>0</v>
+      </c>
+      <c r="N64">
+        <v>0</v>
+      </c>
+      <c r="O64">
+        <v>0</v>
+      </c>
+      <c r="Q64">
+        <v>0</v>
+      </c>
+      <c r="R64">
+        <v>0</v>
+      </c>
+      <c r="S64">
+        <v>0</v>
+      </c>
+      <c r="V64" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W64" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X64" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I65">
+        <v>33342504.4761132</v>
+      </c>
+      <c r="J65">
+        <v>-19138663.946695801</v>
+      </c>
+      <c r="K65">
+        <v>20204.688399999901</v>
+      </c>
+    </row>
+    <row r="66" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I66">
+        <v>33342504.4761132</v>
+      </c>
+      <c r="J66">
+        <v>-19138663.946695801</v>
+      </c>
+      <c r="K66">
+        <v>20204.688399999901</v>
+      </c>
+    </row>
+    <row r="67" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I67">
+        <v>33342504.4761132</v>
+      </c>
+      <c r="J67">
+        <v>-19138663.946695801</v>
+      </c>
+      <c r="K67">
+        <v>6830.6345700000002</v>
+      </c>
+    </row>
+    <row r="68" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I68">
+        <v>33342504.4761132</v>
+      </c>
+      <c r="J68">
+        <v>-19138663.946695801</v>
+      </c>
+      <c r="K68">
+        <v>7508.3215090000003</v>
+      </c>
+    </row>
+    <row r="69" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I69">
+        <v>33342504.4761132</v>
+      </c>
+      <c r="J69">
+        <v>-19138663.946695801</v>
+      </c>
+      <c r="K69">
+        <v>20204.688399999901</v>
+      </c>
+    </row>
+    <row r="70" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I70">
+        <v>33342504.4761132</v>
+      </c>
+      <c r="J70">
+        <v>-19138663.946695801</v>
+      </c>
+      <c r="K70">
+        <v>20204.688399999901</v>
+      </c>
+    </row>
+    <row r="71" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I71">
+        <v>33342504.4761132</v>
+      </c>
+      <c r="J71">
+        <v>-37962582.475577503</v>
+      </c>
+      <c r="K71">
+        <v>20204.688399999901</v>
+      </c>
+    </row>
+    <row r="72" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I72">
+        <v>33342504.4761132</v>
+      </c>
+      <c r="J72">
+        <v>-19138663.946695801</v>
+      </c>
+      <c r="K72">
+        <v>20204.688399999901</v>
+      </c>
+    </row>
+    <row r="73" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I73">
+        <v>33342504.4761132</v>
+      </c>
+      <c r="J73">
+        <v>-19138663.946695801</v>
+      </c>
+      <c r="K73">
+        <v>20204.688399999901</v>
+      </c>
+    </row>
+    <row r="74" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I74">
+        <v>33342504.4761132</v>
+      </c>
+      <c r="J74">
+        <v>-19138663.946695801</v>
+      </c>
+      <c r="K74">
+        <v>20204.688399999901</v>
+      </c>
+    </row>
+    <row r="75" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I75">
+        <v>33342504.4761132</v>
+      </c>
+      <c r="J75">
+        <v>-19138663.946695801</v>
+      </c>
+      <c r="K75">
+        <v>20204.688399999901</v>
+      </c>
+    </row>
+    <row r="76" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I76">
+        <v>33342504.4761132</v>
+      </c>
+      <c r="J76">
+        <v>-19138663.946695801</v>
+      </c>
+      <c r="K76">
+        <v>20204.688399999901</v>
+      </c>
+    </row>
+    <row r="77" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I77">
+        <v>33342504.4761132</v>
+      </c>
+      <c r="J77">
+        <v>-8433986.4392218906</v>
+      </c>
+      <c r="K77">
+        <v>20204.688399999901</v>
+      </c>
+    </row>
+    <row r="78" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I78">
+        <v>33342504.4761132</v>
+      </c>
+      <c r="J78">
+        <v>-19138663.946695801</v>
+      </c>
+      <c r="K78">
+        <v>20204.688399999901</v>
+      </c>
+    </row>
+    <row r="79" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I79">
+        <v>33342504.4761132</v>
+      </c>
+      <c r="J79">
+        <v>-19138663.946695801</v>
+      </c>
+      <c r="K79">
+        <v>20204.688399999901</v>
+      </c>
+    </row>
+    <row r="80" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I80">
+        <v>33342504.4761132</v>
+      </c>
+      <c r="J80">
+        <v>-19138663.946695801</v>
+      </c>
+      <c r="K80">
+        <v>27472.406679999898</v>
+      </c>
+    </row>
+    <row r="81" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I81">
+        <v>33342504.4761132</v>
+      </c>
+      <c r="J81">
+        <v>-19138663.946695801</v>
+      </c>
+      <c r="K81">
+        <v>27472.406679999898</v>
+      </c>
+    </row>
+    <row r="82" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I82">
+        <v>33342504.4761132</v>
+      </c>
+      <c r="J82">
+        <v>-19138663.946695801</v>
+      </c>
+      <c r="K82">
+        <v>27472.406679999898</v>
+      </c>
+    </row>
+    <row r="83" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I83">
+        <v>33342504.4761132</v>
+      </c>
+      <c r="J83">
+        <v>-19138663.946695801</v>
+      </c>
+      <c r="K83">
+        <v>27472.406679999898</v>
+      </c>
+    </row>
+    <row r="84" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I84">
+        <v>33342504.4761132</v>
+      </c>
+      <c r="J84">
+        <v>-19138663.946695801</v>
+      </c>
+      <c r="K84">
+        <v>27472.406679999898</v>
+      </c>
+    </row>
+    <row r="85" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I85">
+        <v>33342504.4761132</v>
+      </c>
+      <c r="J85">
+        <v>-19138663.946695801</v>
+      </c>
+      <c r="K85">
+        <v>27472.406679999898</v>
+      </c>
+    </row>
+    <row r="86" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I86">
+        <v>33342504.4761132</v>
+      </c>
+      <c r="J86">
+        <v>-19138663.946695801</v>
+      </c>
+      <c r="K86">
+        <v>27472.406679999898</v>
+      </c>
+    </row>
+    <row r="87" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I87">
+        <v>33342504.4761132</v>
+      </c>
+      <c r="J87">
+        <v>-19138663.946695801</v>
+      </c>
+      <c r="K87">
+        <v>27472.406679999898</v>
+      </c>
+    </row>
+    <row r="88" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I88">
+        <v>33342504.4761132</v>
+      </c>
+      <c r="J88">
+        <v>-19138663.946695801</v>
+      </c>
+      <c r="K88">
+        <v>27472.406679999898</v>
+      </c>
+    </row>
+    <row r="89" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I89">
+        <v>33342504.4761132</v>
+      </c>
+      <c r="J89">
+        <v>-19138663.946695801</v>
+      </c>
+      <c r="K89">
+        <v>27472.406679999898</v>
+      </c>
+    </row>
+    <row r="90" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I90">
+        <v>33342504.4761132</v>
+      </c>
+      <c r="J90">
+        <v>-19138663.946695801</v>
+      </c>
+      <c r="K90">
+        <v>20204.688399999901</v>
       </c>
     </row>
   </sheetData>

</xml_diff>